<commit_message>
Lab 4 (Add in Test Case Report & Major Changes)
</commit_message>
<xml_diff>
--- a/Lab4/Test Cases & Results/Test Cases.xlsx
+++ b/Lab4/Test Cases & Results/Test Cases.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Junlong\Desktop\Year 2 Sem 1\CZ2006 Software Engineering\Project\CZ2006 Lab 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E14116-7C22-4432-BC25-0503080FC1EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66E7DD9-AACD-484D-B4DE-0134E02D38A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D413FEC8-6CAF-46D1-BD17-CC92A912E122}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D413FEC8-6CAF-46D1-BD17-CC92A912E122}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Account" sheetId="3" r:id="rId1"/>
     <sheet name="Give Clinic Review" sheetId="5" r:id="rId2"/>
-    <sheet name="Notation" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
   <si>
     <t>Input</t>
   </si>
@@ -92,12 +91,6 @@
     <t>Result = False</t>
   </si>
   <si>
-    <t>Not Approved</t>
-  </si>
-  <si>
-    <t>Approved</t>
-  </si>
-  <si>
     <t>Test Title</t>
   </si>
   <si>
@@ -143,54 +136,18 @@
     <t>Password</t>
   </si>
   <si>
-    <t>1, 2, 5, 6, 7, 8, 13, 14</t>
-  </si>
-  <si>
-    <t>a@gmail.com</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
     <t>abc</t>
   </si>
   <si>
-    <t>g@gmail.com</t>
-  </si>
-  <si>
-    <t>gggg</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>1, 2, 5, 6, 7, 8, 9, 10, 11, 9, 10, 12</t>
-  </si>
-  <si>
-    <t>&lt;&lt;NOT APPLICABLE&gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&lt;BLANK&gt;&gt;</t>
-  </si>
-  <si>
     <t>"Account Created" , Profile Page</t>
   </si>
   <si>
     <t>Profile Page</t>
   </si>
   <si>
-    <t>1, 2, 5, 6, 7, 8, 9, 10, 12</t>
-  </si>
-  <si>
-    <t>1, 2, 5, 6, 7, 8, 13, 14, 12</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
     <t>"Wrong Password. Please try again"</t>
   </si>
   <si>
@@ -210,23 +167,73 @@
   </si>
   <si>
     <t>Internet</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Invalid Email</t>
+  </si>
+  <si>
+    <t>Valid Password</t>
+  </si>
+  <si>
+    <t>Valid Existing Email</t>
+  </si>
+  <si>
+    <t>Valid New Email</t>
+  </si>
+  <si>
+    <t>"That email address isn't correct"</t>
+  </si>
+  <si>
+    <t>Valid Gmail Account</t>
+  </si>
+  <si>
+    <t>Gmail Password</t>
+  </si>
+  <si>
+    <t>Wrong Password</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>"Please enter a first and last name"</t>
+  </si>
+  <si>
+    <t>abcdefg</t>
+  </si>
+  <si>
+    <t>"Password not strong enough"</t>
+  </si>
+  <si>
+    <t>1, 2, 6, 7, 8, 10, 11, 12, 5</t>
+  </si>
+  <si>
+    <t>1, 2, 6, 7, 8, 10, 11, 12, 13, 5</t>
+  </si>
+  <si>
+    <t>1, 2, 6, 7, 8, 10, 14, 15, 17, 19, 5</t>
+  </si>
+  <si>
+    <t>1, 2, 6, 7, 8, 9, 7</t>
+  </si>
+  <si>
+    <t>1, 2, 6, 7, 8, 10, 14, 15, 16, 14</t>
+  </si>
+  <si>
+    <t>1, 2, 6, 7, 8, 10, 14, 15, 17, 18, 14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,33 +246,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -280,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -495,12 +482,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -511,68 +653,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,64 +759,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -950,248 +1148,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4280D3-AF64-42A9-9DF2-A059E48F1A19}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="31"/>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="25" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="26"/>
-      <c r="G2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="33"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="46"/>
+      <c r="H7" s="49" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="F8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="50"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="17">
+        <v>2</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="28"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="17">
+        <v>3</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="17">
+        <v>4</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="28"/>
+    </row>
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="17">
+        <v>5</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="41" t="s">
+      <c r="F13" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="17">
+        <v>6</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="28"/>
+    </row>
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="17">
+        <v>7</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="28"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="18">
+        <v>8</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>4</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1" xr:uid="{7DBE0889-F35B-4503-8934-BBC710E01BA6}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{ED89352E-4442-4486-9D83-7606B6945E19}"/>
-    <hyperlink ref="C11" r:id="rId3" xr:uid="{322445BD-2639-4CB6-B2C5-4FEA5AD88865}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{5D2D9100-5E50-4F2D-BAB0-8BCB5D782100}"/>
-    <hyperlink ref="C13" r:id="rId5" xr:uid="{1B227F9A-AB71-4E2B-92A7-573E7E02BB96}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1199,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD262DE0-4F96-4ACE-AE9D-BD4156265460}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1210,116 +1467,115 @@
     <col min="3" max="4" width="11.08984375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="27.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="39"/>
+      <c r="H2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="13">
+        <v>2</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="63"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="25" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="41"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="26"/>
-      <c r="H2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="40">
-        <v>2</v>
-      </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="33"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="32"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="12" t="s">
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14" t="s">
+      <c r="H7" s="46"/>
+      <c r="I7" s="49" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="15"/>
+      <c r="I8" s="50"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="44" t="s">
-        <v>54</v>
+      <c r="B9" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -1343,8 +1599,8 @@
       <c r="A10" s="3">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
-        <v>54</v>
+      <c r="B10" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -1361,15 +1617,15 @@
       <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>3</v>
       </c>
-      <c r="B11" s="44" t="s">
-        <v>54</v>
+      <c r="B11" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
@@ -1386,15 +1642,15 @@
       <c r="G11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>4</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>54</v>
+      <c r="B12" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -1411,15 +1667,15 @@
       <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>5</v>
       </c>
-      <c r="B13" s="44" t="s">
-        <v>54</v>
+      <c r="B13" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
@@ -1436,7 +1692,7 @@
       <c r="G13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1444,7 +1700,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>9</v>
@@ -1469,7 +1725,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
@@ -1494,7 +1750,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>9</v>
@@ -1519,7 +1775,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>9</v>
@@ -1544,7 +1800,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>9</v>
@@ -1569,7 +1825,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>4</v>
@@ -1594,7 +1850,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
@@ -1618,8 +1874,8 @@
       <c r="A21" s="3">
         <v>13</v>
       </c>
-      <c r="B21" s="43" t="s">
-        <v>56</v>
+      <c r="B21" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" ref="C21:F21" si="0">C9</f>
@@ -1636,11 +1892,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G21" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="45"/>
+      <c r="G21" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1661,44 +1917,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1EE928-DD58-4087-8967-CBD244ED86CF}">
-  <dimension ref="B1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="17.54296875" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="28"/>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:B3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed the GetFeedbackForAllClinics in the report
</commit_message>
<xml_diff>
--- a/Lab4/Test Cases & Results/Test Cases.xlsx
+++ b/Lab4/Test Cases & Results/Test Cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CZ2006-Software-Engineering\Lab4\Test Cases &amp; Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\GitHub\CZ2006-Software-Engineering\Lab4\Test Cases &amp; Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DDC23C-B98F-49C5-9BD7-E47FB3144216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Give Clinic Review" sheetId="5" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="34">
   <si>
     <t>Input</t>
   </si>
@@ -129,12 +124,15 @@
   </si>
   <si>
     <t>Result = False("Can't select 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,6 +413,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -442,6 +443,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,18 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -806,34 +804,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="11.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
       <c r="G2" s="4" t="s">
         <v>25</v>
       </c>
@@ -843,60 +845,60 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="36">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24">
         <v>43779</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="19" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16"/>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
@@ -915,9 +917,9 @@
       <c r="G8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -939,11 +941,11 @@
       <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -965,11 +967,11 @@
       <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -991,11 +993,11 @@
       <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -1017,11 +1019,11 @@
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>5</v>
       </c>
@@ -1043,11 +1045,11 @@
       <c r="G13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>6</v>
       </c>
@@ -1069,11 +1071,11 @@
       <c r="G14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>7</v>
       </c>
@@ -1095,11 +1097,11 @@
       <c r="G15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>8</v>
       </c>
@@ -1121,11 +1123,11 @@
       <c r="G16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>9</v>
       </c>
@@ -1147,11 +1149,11 @@
       <c r="G17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>10</v>
       </c>
@@ -1173,11 +1175,11 @@
       <c r="G18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>11</v>
       </c>
@@ -1199,11 +1201,11 @@
       <c r="G19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>12</v>
       </c>
@@ -1225,11 +1227,11 @@
       <c r="G20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>13</v>
       </c>
@@ -1251,11 +1253,11 @@
       <c r="G21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -1277,11 +1279,11 @@
       <c r="G22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -1303,11 +1305,11 @@
       <c r="G23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -1329,11 +1331,11 @@
       <c r="G24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>17</v>
       </c>
@@ -1355,11 +1357,11 @@
       <c r="G25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -1381,11 +1383,11 @@
       <c r="G26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -1407,11 +1409,11 @@
       <c r="G27" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -1433,11 +1435,11 @@
       <c r="G28" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>21</v>
       </c>
@@ -1459,7 +1461,7 @@
       <c r="G29" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="39" t="s">
+      <c r="H29" s="14" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>